<commit_message>
Updating files and adding the 2nd part of the analysis
I decided to divide this analysis into 2 parts, which is why I updated the name of the initial file.

The first part is to analyze the data by "Type", and the second part is to analyze the data by "Tags".

The database had presented a problem with the name of the Tag column, there was a space in the name, so I corrected this problem and updated the document.
</commit_message>
<xml_diff>
--- a/Company_X_Database.xlsx
+++ b/Company_X_Database.xlsx
@@ -4,25 +4,26 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Base" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Planilha Dinamica" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Pivot Table 2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Planilha Dinamica" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Base!$A$1:$J$53</definedName>
   </definedNames>
   <calcPr/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="VHnTpjLpodZJbk5JdQ/jzbSTS4rB4fKnnK+mI+ITLzQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="DdMfNnBJpvTJ7YBkoiA3uFtUKrgGn8rA5rwld7zarz4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="32">
   <si>
     <t>Type</t>
   </si>
@@ -39,7 +40,7 @@
     <t>Views</t>
   </si>
   <si>
-    <t xml:space="preserve">Tags </t>
+    <t>Tags</t>
   </si>
   <si>
     <t>People</t>
@@ -63,7 +64,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>Shop/Products</t>
+    <t>Store/Products</t>
   </si>
   <si>
     <t>Vídeo</t>
@@ -111,10 +112,13 @@
     <t>Commemorative dates/Promotions</t>
   </si>
   <si>
-    <t>Média de Curtidas</t>
+    <t>AVERAGE of Likes</t>
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Média de Curtidas</t>
   </si>
 </sst>
 </file>
@@ -177,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -208,6 +212,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -225,6 +230,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -425,10 +434,10 @@
         <n v="12627.0"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Tags " numFmtId="0">
+    <cacheField name="Tags" numFmtId="0">
       <sharedItems>
         <s v="Store"/>
-        <s v="Shop/Products"/>
+        <s v="Store/Products"/>
         <s v="Products"/>
         <s v="New Products"/>
         <s v="Trends/Products"/>
@@ -521,6 +530,321 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivot Table 2" cacheId="0" dataCaption="" compact="0" compactData="0">
+  <location ref="A1:B6" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields>
+    <pivotField name="Type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField name="Date" compact="0" numFmtId="16" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Likes" dataField="1" compact="0" numFmtId="3" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Comments" compact="0" numFmtId="3" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Views" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Tags" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="People" compact="0" numFmtId="1" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Campaigns" compact="0" numFmtId="1" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Carousel" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Interactions" compact="0" numFmtId="3" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields>
+    <field x="0"/>
+  </rowFields>
+  <dataFields>
+    <dataField name="AVERAGE of Likes" fld="2" subtotal="average" baseField="0"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Planilha Dinamica" cacheId="0" dataCaption="" compact="0" compactData="0">
   <location ref="A3:B8" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields>
@@ -720,7 +1044,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="Tags " compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+    <pivotField name="Tags" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
         <item x="0"/>
         <item x="1"/>
@@ -1056,7 +1380,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1401,7 +1725,7 @@
         <v>13143</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1643,7 +1967,7 @@
         <v>5552</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" hidden="1" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -1943,7 +2267,7 @@
         <v>10055</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" hidden="1" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>10</v>
       </c>
@@ -2210,7 +2534,7 @@
         <v>15576</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" ht="15.75" hidden="1" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>10</v>
       </c>
@@ -2299,7 +2623,7 @@
         <v>21834</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" ht="15.75" hidden="1" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>10</v>
       </c>
@@ -2357,7 +2681,7 @@
         <v>8616</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" ht="15.75" hidden="1" customHeight="1">
       <c r="A45" s="5" t="s">
         <v>10</v>
       </c>
@@ -2537,7 +2861,7 @@
         <v>29563</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" ht="15.75" hidden="1" customHeight="1">
       <c r="A51" s="5" t="s">
         <v>10</v>
       </c>
@@ -2566,7 +2890,7 @@
         <v>9193</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" ht="15.75" hidden="1" customHeight="1">
       <c r="A52" s="5" t="s">
         <v>10</v>
       </c>
@@ -10203,7 +10527,24 @@
       <c r="I1000" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$53"/>
+  <autoFilter ref="$A$1:$J$53">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Influencers"/>
+        <filter val="Products"/>
+        <filter val="Promotions"/>
+        <filter val="Store/Products"/>
+        <filter val="Tips for use/New Products"/>
+        <filter val="Tips for use/Products"/>
+        <filter val="Store"/>
+        <filter val="Commemorative dates/Promotions"/>
+        <filter val="Trends/Products"/>
+        <filter val="Commemorative dates"/>
+        <filter val="New Products"/>
+        <filter val="Trends"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions/>
   <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="portrait"/>
@@ -10212,6 +10553,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+  </sheetData>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>

</xml_diff>